<commit_message>
remove explicit ID from events in timemap setup
</commit_message>
<xml_diff>
--- a/data/timemap_data.xlsx
+++ b/data/timemap_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lachlankermode/code/_fa/datasheet-server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{D1D63EF6-5F28-C941-93D0-C2DD99482839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A957335-1013-C947-AAB9-0599917EF42A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,6 @@
     <sheet name="EXPORT_NARRATIVES" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -181,28 +180,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">The ID can be generated programmatically using the ROW command. ID is required for each event by TimeMap.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">	-Lachlan Kermode</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
       <text>
         <r>
           <rPr>
@@ -223,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -236,7 +214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -257,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -270,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -283,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -296,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -376,7 +354,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="116">
   <si>
     <t>Description</t>
   </si>
@@ -6236,576 +6214,529 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="L1" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="18">
-        <f t="shared" ref="A2:A12" si="0">ROW(A1)</f>
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" t="str">
         <f>Events!A2</f>
         <v>Person A appears on the scene.</v>
       </c>
-      <c r="C2" s="19" t="str">
-        <f>TEXT(Events!B2, "DD/MM/YYYY")</f>
+      <c r="B2" s="19" t="str">
+        <f>TEXT(Events!B2, "MM/DD/YYYY")</f>
         <v>10/10/2015</v>
       </c>
-      <c r="D2" s="20" t="str">
+      <c r="C2" s="20" t="str">
         <f>TEXT(Events!C2, "HH:mm")</f>
         <v>16:20</v>
       </c>
-      <c r="E2" t="str">
+      <c r="D2" t="str">
         <f>Events!D2</f>
         <v>Al Araqib</v>
       </c>
-      <c r="F2">
+      <c r="E2">
         <v>31.3484783</v>
       </c>
-      <c r="G2" s="18">
+      <c r="F2" s="18">
         <v>34.787416899999997</v>
       </c>
-      <c r="H2" s="6" t="str">
+      <c r="G2" s="6" t="str">
         <f>Events!E2</f>
         <v>alpha</v>
       </c>
-      <c r="I2" s="21" t="str">
+      <c r="H2" s="21" t="str">
         <f>IF(ISBLANK(Events!G2), "", Events!G2)</f>
         <v>narrative_1</v>
       </c>
-      <c r="J2" s="21" t="str">
+      <c r="I2" s="21" t="str">
         <f>IF(ISBLANK(Events!H2), "", Events!H2)</f>
         <v>narrative_3</v>
       </c>
-      <c r="K2" s="21" t="str">
+      <c r="J2" s="21" t="str">
         <f>IF(ISBLANK(Events!I2), "", Events!I2)</f>
         <v>src1</v>
       </c>
-      <c r="L2" t="str">
+      <c r="K2" t="str">
         <f>Events!F2</f>
         <v>Person A</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="18">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
         <f>Events!A3</f>
         <v>Person A begins recording.</v>
       </c>
-      <c r="C3" s="19" t="str">
-        <f>TEXT(Events!B3, "DD/MM/YYYY")</f>
+      <c r="B3" s="19" t="str">
+        <f>TEXT(Events!B3, "MM/DD/YYYY")</f>
         <v>10/10/2015</v>
       </c>
-      <c r="D3" s="20" t="str">
+      <c r="C3" s="20" t="str">
         <f>TEXT(Events!C3, "HH:mm")</f>
         <v>16:26</v>
       </c>
-      <c r="E3" t="str">
+      <c r="D3" t="str">
         <f>Events!D3</f>
         <v>Al Araqib</v>
       </c>
-      <c r="F3">
+      <c r="E3">
         <v>31.3484783</v>
       </c>
-      <c r="G3" s="18">
+      <c r="F3" s="18">
         <v>34.787416899999997</v>
       </c>
-      <c r="H3" s="6" t="str">
+      <c r="G3" s="6" t="str">
         <f>Events!E3</f>
         <v>alpha</v>
       </c>
-      <c r="I3" s="21" t="str">
+      <c r="H3" s="21" t="str">
         <f>IF(ISBLANK(Events!G3), "", Events!G3)</f>
         <v>narrative_1</v>
       </c>
-      <c r="J3" s="21" t="str">
+      <c r="I3" s="21" t="str">
         <f>IF(ISBLANK(Events!H3), "", Events!H3)</f>
         <v>narrative_3</v>
       </c>
-      <c r="K3" s="21" t="str">
+      <c r="J3" s="21" t="str">
         <f>IF(ISBLANK(Events!I3), "", Events!I3)</f>
         <v>src2</v>
       </c>
-      <c r="L3" t="str">
+      <c r="K3" t="str">
         <f>Events!F3</f>
         <v>Person A</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="18">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
         <f>Events!A4</f>
         <v>Person B appears in Nahal Pehar, as captured by security footage.</v>
       </c>
-      <c r="C4" s="19" t="str">
-        <f>TEXT(Events!B4, "DD/MM/YYYY")</f>
-        <v>21/10/2015</v>
-      </c>
-      <c r="D4" s="20" t="str">
+      <c r="B4" s="19" t="str">
+        <f>TEXT(Events!B4, "MM/DD/YYYY")</f>
+        <v>10/21/2015</v>
+      </c>
+      <c r="C4" s="20" t="str">
         <f>TEXT(Events!C4, "HH:mm")</f>
         <v>07:00</v>
       </c>
-      <c r="E4" t="str">
+      <c r="D4" t="str">
         <f>Events!D4</f>
         <v>Nahal Pehar</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <v>31.356397000000001</v>
       </c>
-      <c r="G4" s="18">
+      <c r="F4" s="18">
         <v>34.784818000000001</v>
       </c>
-      <c r="H4" s="6" t="str">
+      <c r="G4" s="6" t="str">
         <f>Events!E4</f>
         <v>beta</v>
       </c>
-      <c r="I4" s="21" t="str">
+      <c r="H4" s="21" t="str">
         <f>IF(ISBLANK(Events!G4), "", Events!G4)</f>
         <v>narrative_1</v>
       </c>
-      <c r="J4" s="21" t="str">
+      <c r="I4" s="21" t="str">
         <f>IF(ISBLANK(Events!H4), "", Events!H4)</f>
         <v>narrative_3</v>
       </c>
-      <c r="K4" s="21" t="str">
+      <c r="J4" s="21" t="str">
         <f>IF(ISBLANK(Events!I4), "", Events!I4)</f>
         <v>src6</v>
       </c>
-      <c r="L4" t="str">
+      <c r="K4" t="str">
         <f>Events!F4</f>
         <v>Person B</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" t="str">
         <f>Events!A5</f>
         <v>Fourth thing happened</v>
       </c>
-      <c r="C5" s="19" t="str">
-        <f>TEXT(Events!B5, "DD/MM/YYYY")</f>
-        <v>08/10/2014</v>
-      </c>
-      <c r="D5" s="20" t="str">
+      <c r="B5" s="19" t="str">
+        <f>TEXT(Events!B5, "MM/DD/YYYY")</f>
+        <v>10/08/2014</v>
+      </c>
+      <c r="C5" s="20" t="str">
         <f>TEXT(Events!C5, "HH:mm")</f>
         <v>09:00</v>
       </c>
-      <c r="E5" t="str">
+      <c r="D5" t="str">
         <f>Events!D5</f>
         <v>Tarabin al Tsana</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <v>31.344614499999999</v>
       </c>
-      <c r="G5" s="18">
+      <c r="F5" s="18">
         <v>34.728752299999996</v>
       </c>
-      <c r="H5" s="6" t="str">
+      <c r="G5" s="6" t="str">
         <f>Events!E5</f>
         <v>alpha</v>
       </c>
-      <c r="I5" s="21" t="str">
+      <c r="H5" s="21" t="str">
         <f>IF(ISBLANK(Events!G5), "", Events!G5)</f>
         <v>narrative_2</v>
       </c>
-      <c r="J5" s="21" t="str">
+      <c r="I5" s="21" t="str">
         <f>IF(ISBLANK(Events!H5), "", Events!H5)</f>
         <v/>
       </c>
-      <c r="K5" s="21" t="str">
+      <c r="J5" s="21" t="str">
         <f>IF(ISBLANK(Events!I5), "", Events!I5)</f>
         <v>src5</v>
       </c>
-      <c r="L5" t="str">
+      <c r="K5" t="str">
         <f>Events!F5</f>
         <v>Context</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="18">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" t="str">
         <f>Events!A6</f>
         <v>Fifth thing happened</v>
       </c>
-      <c r="C6" s="19" t="str">
-        <f>TEXT(Events!B6, "DD/MM/YYYY")</f>
-        <v>08/11/2014</v>
-      </c>
-      <c r="D6" s="20" t="str">
+      <c r="B6" s="19" t="str">
+        <f>TEXT(Events!B6, "MM/DD/YYYY")</f>
+        <v>11/08/2014</v>
+      </c>
+      <c r="C6" s="20" t="str">
         <f>TEXT(Events!C6, "HH:mm")</f>
         <v>09:00</v>
       </c>
-      <c r="E6" t="str">
+      <c r="D6" t="str">
         <f>Events!D6</f>
         <v>Mishmar HaNegev</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <v>31.364087099999999</v>
       </c>
-      <c r="G6" s="18">
+      <c r="F6" s="18">
         <v>34.713539599999997</v>
       </c>
-      <c r="H6" s="6" t="str">
+      <c r="G6" s="6" t="str">
         <f>Events!E6</f>
         <v>alpha</v>
       </c>
-      <c r="I6" s="21" t="str">
+      <c r="H6" s="21" t="str">
         <f>IF(ISBLANK(Events!G6), "", Events!G6)</f>
         <v>narrative_2</v>
       </c>
-      <c r="J6" s="21" t="str">
+      <c r="I6" s="21" t="str">
         <f>IF(ISBLANK(Events!H6), "", Events!H6)</f>
         <v/>
       </c>
-      <c r="K6" s="21" t="str">
+      <c r="J6" s="21" t="str">
         <f>IF(ISBLANK(Events!I6), "", Events!I6)</f>
         <v>src7</v>
       </c>
-      <c r="L6" t="str">
+      <c r="K6" t="str">
         <f>Events!F6</f>
         <v>Context</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" t="str">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" t="str">
         <f>Events!A7</f>
         <v>Sixth thing happened</v>
       </c>
-      <c r="C7" s="19" t="str">
-        <f>TEXT(Events!B7, "DD/MM/YYYY")</f>
-        <v>09/12/2014</v>
-      </c>
-      <c r="D7" s="20" t="str">
+      <c r="B7" s="19" t="str">
+        <f>TEXT(Events!B7, "MM/DD/YYYY")</f>
+        <v>12/09/2014</v>
+      </c>
+      <c r="C7" s="20" t="str">
         <f>TEXT(Events!C7, "HH:mm")</f>
         <v>12:00</v>
       </c>
-      <c r="E7" t="str">
+      <c r="D7" t="str">
         <f>Events!D7</f>
         <v>Duda'im Forest</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <v>31.344051400000001</v>
       </c>
-      <c r="G7" s="18">
+      <c r="F7" s="18">
         <v>34.7616005</v>
       </c>
-      <c r="H7" s="6" t="str">
+      <c r="G7" s="6" t="str">
         <f>Events!E7</f>
         <v>alpha</v>
       </c>
-      <c r="I7" s="21" t="str">
+      <c r="H7" s="21" t="str">
         <f>IF(ISBLANK(Events!G7), "", Events!G7)</f>
         <v>narrative_2</v>
       </c>
-      <c r="J7" s="21" t="str">
+      <c r="I7" s="21" t="str">
         <f>IF(ISBLANK(Events!H7), "", Events!H7)</f>
         <v/>
       </c>
-      <c r="K7" s="21" t="str">
+      <c r="J7" s="21" t="str">
         <f>IF(ISBLANK(Events!I7), "", Events!I7)</f>
         <v>src7</v>
       </c>
-      <c r="L7" t="str">
+      <c r="K7" t="str">
         <f>Events!F7</f>
         <v>Context</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="18">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" t="str">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" t="str">
         <f>Events!A8</f>
         <v>Seventh thing happened (out of space)</v>
       </c>
-      <c r="C8" s="19" t="str">
-        <f>TEXT(Events!B8, "DD/MM/YYYY")</f>
-        <v>10/12/2014</v>
-      </c>
-      <c r="D8" s="20" t="str">
+      <c r="B8" s="19" t="str">
+        <f>TEXT(Events!B8, "MM/DD/YYYY")</f>
+        <v>12/10/2014</v>
+      </c>
+      <c r="C8" s="20" t="str">
         <f>TEXT(Events!C8, "HH:mm")</f>
         <v>01:00</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
         <v>114</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="H8" s="6" t="str">
+      <c r="G8" s="6" t="str">
         <f>Events!E8</f>
         <v>beta</v>
       </c>
-      <c r="I8" s="21" t="str">
+      <c r="H8" s="21" t="str">
         <f>IF(ISBLANK(Events!G8), "", Events!G8)</f>
         <v>narrative_3</v>
       </c>
-      <c r="J8" s="21" t="str">
+      <c r="I8" s="21" t="str">
         <f>IF(ISBLANK(Events!H8), "", Events!H8)</f>
         <v/>
       </c>
-      <c r="K8" s="21" t="str">
+      <c r="J8" s="21" t="str">
         <f>IF(ISBLANK(Events!I8), "", Events!I8)</f>
         <v>src4</v>
       </c>
-      <c r="L8" t="str">
+      <c r="K8" t="str">
         <f>Events!F8</f>
         <v>Context</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="18">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" t="str">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" t="str">
         <f>Events!A9</f>
         <v>8th thing happened</v>
       </c>
-      <c r="C9" s="19" t="str">
-        <f>TEXT(Events!B9, "DD/MM/YYYY")</f>
-        <v>09/12/2014</v>
-      </c>
-      <c r="D9" s="20" t="str">
+      <c r="B9" s="19" t="str">
+        <f>TEXT(Events!B9, "MM/DD/YYYY")</f>
+        <v>12/09/2014</v>
+      </c>
+      <c r="C9" s="20" t="str">
         <f>TEXT(Events!C9, "HH:mm")</f>
         <v>11:00</v>
       </c>
-      <c r="E9" t="str">
+      <c r="D9" t="str">
         <f>Events!D9</f>
         <v>Nahal Duda'im</v>
       </c>
-      <c r="F9">
+      <c r="E9">
         <v>31.342402700000001</v>
       </c>
-      <c r="G9" s="18">
+      <c r="F9" s="18">
         <v>34.790981100000003</v>
       </c>
-      <c r="H9" s="6" t="str">
+      <c r="G9" s="6" t="str">
         <f>Events!E9</f>
         <v>alpha</v>
       </c>
-      <c r="I9" s="21" t="str">
+      <c r="H9" s="21" t="str">
         <f>IF(ISBLANK(Events!G9), "", Events!G9)</f>
         <v>narrative_1</v>
       </c>
-      <c r="J9" s="21" t="str">
+      <c r="I9" s="21" t="str">
         <f>IF(ISBLANK(Events!H9), "", Events!H9)</f>
         <v/>
       </c>
-      <c r="K9" s="21" t="str">
+      <c r="J9" s="21" t="str">
         <f>IF(ISBLANK(Events!I9), "", Events!I9)</f>
         <v>src5</v>
       </c>
-      <c r="L9" t="str">
+      <c r="K9" t="str">
         <f>Events!F9</f>
         <v>Context</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="18">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" t="str">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" t="str">
         <f>Events!A10</f>
         <v>9th thing happened</v>
       </c>
-      <c r="C10" s="19" t="str">
-        <f>TEXT(Events!B10, "DD/MM/YYYY")</f>
-        <v>09/12/2014</v>
-      </c>
-      <c r="D10" s="20" t="str">
+      <c r="B10" s="19" t="str">
+        <f>TEXT(Events!B10, "MM/DD/YYYY")</f>
+        <v>12/09/2014</v>
+      </c>
+      <c r="C10" s="20" t="str">
         <f>TEXT(Events!C10, "HH:mm")</f>
         <v>11:00</v>
       </c>
-      <c r="E10" t="str">
+      <c r="D10" t="str">
         <f>Events!D10</f>
         <v>Nahal Pehar</v>
       </c>
-      <c r="F10">
+      <c r="E10">
         <v>31.356397000000001</v>
       </c>
-      <c r="G10" s="18">
+      <c r="F10" s="18">
         <v>34.784818000000001</v>
       </c>
-      <c r="H10" s="6" t="str">
+      <c r="G10" s="6" t="str">
         <f>Events!E10</f>
         <v>alpha</v>
       </c>
-      <c r="I10" s="21" t="str">
+      <c r="H10" s="21" t="str">
         <f>IF(ISBLANK(Events!G10), "", Events!G10)</f>
         <v>narrative_2</v>
       </c>
-      <c r="J10" s="21" t="str">
+      <c r="I10" s="21" t="str">
         <f>IF(ISBLANK(Events!H10), "", Events!H10)</f>
         <v/>
       </c>
-      <c r="K10" s="21" t="str">
+      <c r="J10" s="21" t="str">
         <f>IF(ISBLANK(Events!I10), "", Events!I10)</f>
         <v>src3</v>
       </c>
-      <c r="L10" t="str">
+      <c r="K10" t="str">
         <f>Events!F10</f>
         <v>Context</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="18">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" t="str">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" t="str">
         <f>Events!A11</f>
         <v>10th thing happened</v>
       </c>
-      <c r="C11" s="19" t="str">
-        <f>TEXT(Events!B11, "DD/MM/YYYY")</f>
-        <v>09/11/2014</v>
-      </c>
-      <c r="D11" s="20" t="str">
+      <c r="B11" s="19" t="str">
+        <f>TEXT(Events!B11, "MM/DD/YYYY")</f>
+        <v>11/09/2014</v>
+      </c>
+      <c r="C11" s="20" t="str">
         <f>TEXT(Events!C11, "HH:mm")</f>
         <v>10:48</v>
       </c>
-      <c r="E11" t="str">
+      <c r="D11" t="str">
         <f>Events!D11</f>
         <v>Nahal Pehar</v>
       </c>
-      <c r="F11">
+      <c r="E11">
         <v>31.356397000000001</v>
       </c>
-      <c r="G11" s="18">
+      <c r="F11" s="18">
         <v>34.784818000000001</v>
       </c>
-      <c r="H11" s="6" t="str">
+      <c r="G11" s="6" t="str">
         <f>Events!E11</f>
         <v>alpha</v>
       </c>
-      <c r="I11" s="21" t="str">
+      <c r="H11" s="21" t="str">
         <f>IF(ISBLANK(Events!G11), "", Events!G11)</f>
         <v/>
       </c>
-      <c r="J11" s="21" t="str">
+      <c r="I11" s="21" t="str">
         <f>IF(ISBLANK(Events!H11), "", Events!H11)</f>
         <v/>
       </c>
-      <c r="K11" s="21" t="str">
+      <c r="J11" s="21" t="str">
         <f>IF(ISBLANK(Events!I11), "", Events!I11)</f>
         <v>src6</v>
       </c>
-      <c r="L11" t="str">
+      <c r="K11" t="str">
         <f>Events!F11</f>
         <v>Context</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="18">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" t="str">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" t="str">
         <f>Events!A12</f>
         <v>11th thing happened</v>
       </c>
-      <c r="C12" s="19" t="str">
-        <f>TEXT(Events!B12, "DD/MM/YYYY")</f>
-        <v>30/11/2014</v>
-      </c>
-      <c r="D12" s="20" t="str">
+      <c r="B12" s="19" t="str">
+        <f>TEXT(Events!B12, "MM/DD/YYYY")</f>
+        <v>11/30/2014</v>
+      </c>
+      <c r="C12" s="20" t="str">
         <f>TEXT(Events!C12, "HH:mm")</f>
         <v>11:00</v>
       </c>
-      <c r="E12" t="str">
+      <c r="D12" t="str">
         <f>Events!D12</f>
         <v>Tarabin al Tsana</v>
       </c>
-      <c r="F12">
+      <c r="E12">
         <v>31.344614499999999</v>
       </c>
-      <c r="G12" s="18">
+      <c r="F12" s="18">
         <v>34.728752299999996</v>
       </c>
-      <c r="H12" s="6" t="str">
+      <c r="G12" s="6" t="str">
         <f>Events!E12</f>
         <v>beta</v>
       </c>
-      <c r="I12" s="21" t="str">
+      <c r="H12" s="21" t="str">
         <f>IF(ISBLANK(Events!G12), "", Events!G12)</f>
         <v>narrative_3</v>
       </c>
-      <c r="J12" s="21" t="str">
+      <c r="I12" s="21" t="str">
         <f>IF(ISBLANK(Events!H12), "", Events!H12)</f>
         <v/>
       </c>
-      <c r="K12" s="21" t="str">
+      <c r="J12" s="21" t="str">
         <f>IF(ISBLANK(Events!I12), "", Events!I12)</f>
         <v>src8</v>
       </c>
-      <c r="L12" t="str">
+      <c r="K12" t="str">
         <f>Events!F12</f>
         <v>Context</v>
       </c>

</xml_diff>

<commit_message>
Collapsed filters and narratives into associations; modified default tabs to reflect
</commit_message>
<xml_diff>
--- a/data/timemap_data.xlsx
+++ b/data/timemap_data.xlsx
@@ -1,42 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lachlankermode/code/_fa/datasheet-server/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/efarooqui/Desktop/FA/datasheet-server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783DD13B-71D9-C241-AE6F-E81E732AEEFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F3A32D-6F32-4743-AC80-07CEFB13A59C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3100" yWindow="1640" windowWidth="28800" windowHeight="18000" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
-    <sheet name="Sources" sheetId="2" r:id="rId2"/>
-    <sheet name="Filters" sheetId="3" r:id="rId3"/>
-    <sheet name="Narratives" sheetId="4" r:id="rId4"/>
-    <sheet name="Categories" sheetId="5" r:id="rId5"/>
-    <sheet name="Locations" sheetId="6" r:id="rId6"/>
-    <sheet name="EXPORT_EVENTS" sheetId="7" r:id="rId7"/>
-    <sheet name="EXPORT_CATEGORIES" sheetId="8" r:id="rId8"/>
-    <sheet name="EXPORT_SOURCES" sheetId="9" r:id="rId9"/>
-    <sheet name="EXPORT_FILTERS" sheetId="10" r:id="rId10"/>
-    <sheet name="EXPORT_SITES" sheetId="11" r:id="rId11"/>
-    <sheet name="EXPORT_NARRATIVES" sheetId="12" r:id="rId12"/>
+    <sheet name="Associations" sheetId="13" r:id="rId2"/>
+    <sheet name="Sources" sheetId="2" r:id="rId3"/>
+    <sheet name="Categories" sheetId="5" r:id="rId4"/>
+    <sheet name="Sites" sheetId="6" r:id="rId5"/>
+    <sheet name="EXPORT_EVENTS" sheetId="7" r:id="rId6"/>
+    <sheet name="EXPORT_CATEGORIES" sheetId="8" r:id="rId7"/>
+    <sheet name="EXPORT_SOURCES" sheetId="9" r:id="rId8"/>
+    <sheet name="EXPORT_ASSOCIATIONS" sheetId="10" r:id="rId9"/>
+    <sheet name="EXPORT_SITES" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -323,7 +311,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="129">
   <si>
     <t>Description</t>
   </si>
@@ -406,9 +394,6 @@
     <t>Tarabin al Tsana</t>
   </si>
   <si>
-    <t>Context</t>
-  </si>
-  <si>
     <t>narrative_2</t>
   </si>
   <si>
@@ -577,21 +562,6 @@
     <t>non_existent.md</t>
   </si>
   <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>An explanation of narrative 1</t>
-  </si>
-  <si>
-    <t>An explanation of narrative 2</t>
-  </si>
-  <si>
-    <t>Narrative 3</t>
-  </si>
-  <si>
-    <t>An explanation of narrative 3</t>
-  </si>
-  <si>
     <t>Of highest priority</t>
   </si>
   <si>
@@ -658,19 +628,76 @@
     <t>site</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>tag1</t>
   </si>
   <si>
-    <t>People</t>
-  </si>
-  <si>
     <t>Unaffiliated</t>
+  </si>
+  <si>
+    <t>Narrative</t>
+  </si>
+  <si>
+    <t>Weapons</t>
+  </si>
+  <si>
+    <t>tear gas</t>
+  </si>
+  <si>
+    <t>pistol</t>
+  </si>
+  <si>
+    <t>rifle</t>
+  </si>
+  <si>
+    <t>baton</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Close Range</t>
+  </si>
+  <si>
+    <t>Long Range</t>
+  </si>
+  <si>
+    <t>Filter Path</t>
+  </si>
+  <si>
+    <t>canisters</t>
+  </si>
+  <si>
+    <t>gun</t>
+  </si>
+  <si>
+    <t>melee</t>
+  </si>
+  <si>
+    <t>first narrative</t>
+  </si>
+  <si>
+    <t>second narrative</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>filter_path0</t>
+  </si>
+  <si>
+    <t>filter_path1</t>
+  </si>
+  <si>
+    <t>filter_path2</t>
   </si>
 </sst>
 </file>
@@ -683,7 +710,7 @@
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="167" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -731,6 +758,30 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -740,7 +791,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -748,20 +799,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -786,8 +828,6 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -795,6 +835,10 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,7 +1158,7 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F5" sqref="F5:F12"/>
     </sheetView>
@@ -1269,20 +1313,20 @@
         <v>12</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="10">
         <v>41951</v>
@@ -1291,26 +1335,26 @@
         <v>0.375</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="10">
         <v>41982</v>
@@ -1319,26 +1363,26 @@
         <v>0.5</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="12">
         <v>41983</v>
@@ -1350,22 +1394,22 @@
         <v>22</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="10">
         <v>41982</v>
@@ -1374,26 +1418,26 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="10">
         <v>41982</v>
@@ -1408,20 +1452,20 @@
         <v>12</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="10">
         <v>41952</v>
@@ -1436,18 +1480,18 @@
         <v>12</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>24</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="10">
         <v>41973</v>
@@ -1462,13 +1506,13 @@
         <v>22</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J12" s="8"/>
     </row>
@@ -5438,19 +5482,19 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
-            <xm:f>Locations!$A$2:$A$1000</xm:f>
+            <xm:f>Sites!$A$2:$A$1000</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
-            <xm:f>Narratives!$A$2:$A$1000</xm:f>
+            <xm:f>#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G2:H1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
-            <xm:f>Filters!$A:$A</xm:f>
+            <xm:f>#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1000</xm:sqref>
         </x14:dataValidation>
@@ -5467,53 +5511,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="str">
-        <f>IF(ISBLANK(Filters!A1), "", Filters!A1)</f>
-        <v>Context</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="str">
-        <f>IF(ISBLANK(Filters!A2), "", Filters!A2)</f>
-        <v>People</v>
-      </c>
-      <c r="B2" s="6" t="str">
-        <f>IF(ISBLANK(Filters!B2), "", Filters!B2)</f>
-        <v>Person A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="str">
-        <f>IF(ISBLANK(Filters!A3), "", Filters!A3)</f>
-        <v>People</v>
-      </c>
-      <c r="B3" s="6" t="str">
-        <f>IF(ISBLANK(Filters!B3), "", Filters!B3)</f>
-        <v>Person B</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5522,65 +5519,65 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="16"/>
+      <c r="F1" s="14"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="21">
+      <c r="A2" s="19">
         <f>ROW(A1)</f>
         <v>1</v>
       </c>
       <c r="C2" t="str">
-        <f>Locations!A3</f>
+        <f>Sites!A3</f>
         <v>Nahal Pehar</v>
       </c>
       <c r="D2">
-        <f>Locations!B3</f>
+        <f>Sites!B3</f>
         <v>31.356397000000001</v>
       </c>
       <c r="E2">
-        <f>Locations!C3</f>
+        <f>Sites!C3</f>
         <v>34.784818000000001</v>
       </c>
     </row>
@@ -5590,83 +5587,122 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:Z4"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A93F27E4-DD3D-8649-A0D0-A294CC3CFBB3}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="B3" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>88</v>
+      <c r="B6" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -5674,7 +5710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5694,28 +5730,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5723,19 +5759,19 @@
         <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5743,83 +5779,83 @@
         <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5827,59 +5863,59 @@
         <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5896,130 +5932,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:Z4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6035,42 +5948,42 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6078,7 +5991,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -6086,7 +5999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6095,20 +6008,20 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>9</v>
@@ -6138,7 +6051,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="6">
         <v>31.342402700000001</v>
@@ -6160,7 +6073,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6">
         <v>31.364087099999999</v>
@@ -6171,7 +6084,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="6">
         <v>31.344051400000001</v>
@@ -6185,7 +6098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6194,7 +6107,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6204,37 +6117,37 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6242,11 +6155,11 @@
         <f>Events!A2</f>
         <v>Person A appears on the scene.</v>
       </c>
-      <c r="B2" s="19" t="str">
+      <c r="B2" s="17" t="str">
         <f>TEXT(Events!B2, "MM/DD/YYYY")</f>
         <v>10/10/2015</v>
       </c>
-      <c r="C2" s="20" t="str">
+      <c r="C2" s="18" t="str">
         <f>TEXT(Events!C2, "HH:mm")</f>
         <v>16:20</v>
       </c>
@@ -6257,22 +6170,22 @@
       <c r="E2">
         <v>31.3484783</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="16">
         <v>34.787416899999997</v>
       </c>
       <c r="G2" s="6" t="str">
         <f>Events!E2</f>
         <v>alpha</v>
       </c>
-      <c r="H2" s="21" t="str">
+      <c r="H2" s="19" t="str">
         <f>IF(ISBLANK(Events!G2), "", Events!G2)</f>
         <v>narrative_1</v>
       </c>
-      <c r="I2" s="21" t="str">
+      <c r="I2" s="19" t="str">
         <f>IF(ISBLANK(Events!H2), "", Events!H2)</f>
         <v>narrative_3</v>
       </c>
-      <c r="J2" s="21" t="str">
+      <c r="J2" s="19" t="str">
         <f>IF(ISBLANK(Events!I2), "", Events!I2)</f>
         <v>src1</v>
       </c>
@@ -6286,11 +6199,11 @@
         <f>Events!A3</f>
         <v>Person A begins recording.</v>
       </c>
-      <c r="B3" s="19" t="str">
+      <c r="B3" s="17" t="str">
         <f>TEXT(Events!B3, "MM/DD/YYYY")</f>
         <v>10/10/2015</v>
       </c>
-      <c r="C3" s="20" t="str">
+      <c r="C3" s="18" t="str">
         <f>TEXT(Events!C3, "HH:mm")</f>
         <v>16:26</v>
       </c>
@@ -6301,22 +6214,22 @@
       <c r="E3">
         <v>31.3484783</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="16">
         <v>34.787416899999997</v>
       </c>
       <c r="G3" s="6" t="str">
         <f>Events!E3</f>
         <v>alpha</v>
       </c>
-      <c r="H3" s="21" t="str">
+      <c r="H3" s="19" t="str">
         <f>IF(ISBLANK(Events!G3), "", Events!G3)</f>
         <v>narrative_1</v>
       </c>
-      <c r="I3" s="21" t="str">
+      <c r="I3" s="19" t="str">
         <f>IF(ISBLANK(Events!H3), "", Events!H3)</f>
         <v>narrative_3</v>
       </c>
-      <c r="J3" s="21" t="str">
+      <c r="J3" s="19" t="str">
         <f>IF(ISBLANK(Events!I3), "", Events!I3)</f>
         <v>src2</v>
       </c>
@@ -6330,11 +6243,11 @@
         <f>Events!A4</f>
         <v>Person B appears in Nahal Pehar, as captured by security footage.</v>
       </c>
-      <c r="B4" s="19" t="str">
+      <c r="B4" s="17" t="str">
         <f>TEXT(Events!B4, "MM/DD/YYYY")</f>
         <v>10/21/2015</v>
       </c>
-      <c r="C4" s="20" t="str">
+      <c r="C4" s="18" t="str">
         <f>TEXT(Events!C4, "HH:mm")</f>
         <v>07:00</v>
       </c>
@@ -6345,22 +6258,22 @@
       <c r="E4">
         <v>31.356397000000001</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="16">
         <v>34.784818000000001</v>
       </c>
       <c r="G4" s="6" t="str">
         <f>Events!E4</f>
         <v>beta</v>
       </c>
-      <c r="H4" s="21" t="str">
+      <c r="H4" s="19" t="str">
         <f>IF(ISBLANK(Events!G4), "", Events!G4)</f>
         <v>narrative_1</v>
       </c>
-      <c r="I4" s="21" t="str">
+      <c r="I4" s="19" t="str">
         <f>IF(ISBLANK(Events!H4), "", Events!H4)</f>
         <v>narrative_3</v>
       </c>
-      <c r="J4" s="21" t="str">
+      <c r="J4" s="19" t="str">
         <f>IF(ISBLANK(Events!I4), "", Events!I4)</f>
         <v>src6</v>
       </c>
@@ -6374,11 +6287,11 @@
         <f>Events!A5</f>
         <v>Fourth thing happened</v>
       </c>
-      <c r="B5" s="19" t="str">
+      <c r="B5" s="17" t="str">
         <f>TEXT(Events!B5, "MM/DD/YYYY")</f>
         <v>10/08/2014</v>
       </c>
-      <c r="C5" s="20" t="str">
+      <c r="C5" s="18" t="str">
         <f>TEXT(Events!C5, "HH:mm")</f>
         <v>09:00</v>
       </c>
@@ -6389,22 +6302,22 @@
       <c r="E5">
         <v>31.344614499999999</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="16">
         <v>34.728752299999996</v>
       </c>
       <c r="G5" s="6" t="str">
         <f>Events!E5</f>
         <v>alpha</v>
       </c>
-      <c r="H5" s="21" t="str">
+      <c r="H5" s="19" t="str">
         <f>IF(ISBLANK(Events!G5), "", Events!G5)</f>
         <v>narrative_2</v>
       </c>
-      <c r="I5" s="21" t="str">
+      <c r="I5" s="19" t="str">
         <f>IF(ISBLANK(Events!H5), "", Events!H5)</f>
         <v/>
       </c>
-      <c r="J5" s="21" t="str">
+      <c r="J5" s="19" t="str">
         <f>IF(ISBLANK(Events!I5), "", Events!I5)</f>
         <v>src5</v>
       </c>
@@ -6418,11 +6331,11 @@
         <f>Events!A6</f>
         <v>Fifth thing happened</v>
       </c>
-      <c r="B6" s="19" t="str">
+      <c r="B6" s="17" t="str">
         <f>TEXT(Events!B6, "MM/DD/YYYY")</f>
         <v>11/08/2014</v>
       </c>
-      <c r="C6" s="20" t="str">
+      <c r="C6" s="18" t="str">
         <f>TEXT(Events!C6, "HH:mm")</f>
         <v>09:00</v>
       </c>
@@ -6433,22 +6346,22 @@
       <c r="E6">
         <v>31.364087099999999</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="16">
         <v>34.713539599999997</v>
       </c>
       <c r="G6" s="6" t="str">
         <f>Events!E6</f>
         <v>alpha</v>
       </c>
-      <c r="H6" s="21" t="str">
+      <c r="H6" s="19" t="str">
         <f>IF(ISBLANK(Events!G6), "", Events!G6)</f>
         <v>narrative_2</v>
       </c>
-      <c r="I6" s="21" t="str">
+      <c r="I6" s="19" t="str">
         <f>IF(ISBLANK(Events!H6), "", Events!H6)</f>
         <v/>
       </c>
-      <c r="J6" s="21" t="str">
+      <c r="J6" s="19" t="str">
         <f>IF(ISBLANK(Events!I6), "", Events!I6)</f>
         <v>src7</v>
       </c>
@@ -6462,11 +6375,11 @@
         <f>Events!A7</f>
         <v>Sixth thing happened</v>
       </c>
-      <c r="B7" s="19" t="str">
+      <c r="B7" s="17" t="str">
         <f>TEXT(Events!B7, "MM/DD/YYYY")</f>
         <v>12/09/2014</v>
       </c>
-      <c r="C7" s="20" t="str">
+      <c r="C7" s="18" t="str">
         <f>TEXT(Events!C7, "HH:mm")</f>
         <v>12:00</v>
       </c>
@@ -6477,22 +6390,22 @@
       <c r="E7">
         <v>31.344051400000001</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <v>34.7616005</v>
       </c>
       <c r="G7" s="6" t="str">
         <f>Events!E7</f>
         <v>alpha</v>
       </c>
-      <c r="H7" s="21" t="str">
+      <c r="H7" s="19" t="str">
         <f>IF(ISBLANK(Events!G7), "", Events!G7)</f>
         <v>narrative_2</v>
       </c>
-      <c r="I7" s="21" t="str">
+      <c r="I7" s="19" t="str">
         <f>IF(ISBLANK(Events!H7), "", Events!H7)</f>
         <v/>
       </c>
-      <c r="J7" s="21" t="str">
+      <c r="J7" s="19" t="str">
         <f>IF(ISBLANK(Events!I7), "", Events!I7)</f>
         <v>src7</v>
       </c>
@@ -6506,33 +6419,33 @@
         <f>Events!A8</f>
         <v>Seventh thing happened (out of space)</v>
       </c>
-      <c r="B8" s="19" t="str">
+      <c r="B8" s="17" t="str">
         <f>TEXT(Events!B8, "MM/DD/YYYY")</f>
         <v>12/10/2014</v>
       </c>
-      <c r="C8" s="20" t="str">
+      <c r="C8" s="18" t="str">
         <f>TEXT(Events!C8, "HH:mm")</f>
         <v>01:00</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>112</v>
+        <v>105</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>105</v>
       </c>
       <c r="G8" s="6" t="str">
         <f>Events!E8</f>
         <v>beta</v>
       </c>
-      <c r="H8" s="21" t="str">
+      <c r="H8" s="19" t="str">
         <f>IF(ISBLANK(Events!G8), "", Events!G8)</f>
         <v>narrative_3</v>
       </c>
-      <c r="I8" s="21" t="str">
+      <c r="I8" s="19" t="str">
         <f>IF(ISBLANK(Events!H8), "", Events!H8)</f>
         <v/>
       </c>
-      <c r="J8" s="21" t="str">
+      <c r="J8" s="19" t="str">
         <f>IF(ISBLANK(Events!I8), "", Events!I8)</f>
         <v>src4</v>
       </c>
@@ -6546,11 +6459,11 @@
         <f>Events!A9</f>
         <v>8th thing happened</v>
       </c>
-      <c r="B9" s="19" t="str">
+      <c r="B9" s="17" t="str">
         <f>TEXT(Events!B9, "MM/DD/YYYY")</f>
         <v>12/09/2014</v>
       </c>
-      <c r="C9" s="20" t="str">
+      <c r="C9" s="18" t="str">
         <f>TEXT(Events!C9, "HH:mm")</f>
         <v>11:00</v>
       </c>
@@ -6561,22 +6474,22 @@
       <c r="E9">
         <v>31.342402700000001</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="16">
         <v>34.790981100000003</v>
       </c>
       <c r="G9" s="6" t="str">
         <f>Events!E9</f>
         <v>alpha</v>
       </c>
-      <c r="H9" s="21" t="str">
+      <c r="H9" s="19" t="str">
         <f>IF(ISBLANK(Events!G9), "", Events!G9)</f>
         <v>narrative_1</v>
       </c>
-      <c r="I9" s="21" t="str">
+      <c r="I9" s="19" t="str">
         <f>IF(ISBLANK(Events!H9), "", Events!H9)</f>
         <v/>
       </c>
-      <c r="J9" s="21" t="str">
+      <c r="J9" s="19" t="str">
         <f>IF(ISBLANK(Events!I9), "", Events!I9)</f>
         <v>src5</v>
       </c>
@@ -6590,11 +6503,11 @@
         <f>Events!A10</f>
         <v>9th thing happened</v>
       </c>
-      <c r="B10" s="19" t="str">
+      <c r="B10" s="17" t="str">
         <f>TEXT(Events!B10, "MM/DD/YYYY")</f>
         <v>12/09/2014</v>
       </c>
-      <c r="C10" s="20" t="str">
+      <c r="C10" s="18" t="str">
         <f>TEXT(Events!C10, "HH:mm")</f>
         <v>11:00</v>
       </c>
@@ -6605,22 +6518,22 @@
       <c r="E10">
         <v>31.356397000000001</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <v>34.784818000000001</v>
       </c>
       <c r="G10" s="6" t="str">
         <f>Events!E10</f>
         <v>alpha</v>
       </c>
-      <c r="H10" s="21" t="str">
+      <c r="H10" s="19" t="str">
         <f>IF(ISBLANK(Events!G10), "", Events!G10)</f>
         <v>narrative_2</v>
       </c>
-      <c r="I10" s="21" t="str">
+      <c r="I10" s="19" t="str">
         <f>IF(ISBLANK(Events!H10), "", Events!H10)</f>
         <v/>
       </c>
-      <c r="J10" s="21" t="str">
+      <c r="J10" s="19" t="str">
         <f>IF(ISBLANK(Events!I10), "", Events!I10)</f>
         <v>src3</v>
       </c>
@@ -6634,11 +6547,11 @@
         <f>Events!A11</f>
         <v>10th thing happened</v>
       </c>
-      <c r="B11" s="19" t="str">
+      <c r="B11" s="17" t="str">
         <f>TEXT(Events!B11, "MM/DD/YYYY")</f>
         <v>11/09/2014</v>
       </c>
-      <c r="C11" s="20" t="str">
+      <c r="C11" s="18" t="str">
         <f>TEXT(Events!C11, "HH:mm")</f>
         <v>10:48</v>
       </c>
@@ -6649,22 +6562,22 @@
       <c r="E11">
         <v>31.356397000000001</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <v>34.784818000000001</v>
       </c>
       <c r="G11" s="6" t="str">
         <f>Events!E11</f>
         <v>alpha</v>
       </c>
-      <c r="H11" s="21" t="str">
+      <c r="H11" s="19" t="str">
         <f>IF(ISBLANK(Events!G11), "", Events!G11)</f>
         <v/>
       </c>
-      <c r="I11" s="21" t="str">
+      <c r="I11" s="19" t="str">
         <f>IF(ISBLANK(Events!H11), "", Events!H11)</f>
         <v/>
       </c>
-      <c r="J11" s="21" t="str">
+      <c r="J11" s="19" t="str">
         <f>IF(ISBLANK(Events!I11), "", Events!I11)</f>
         <v>src6</v>
       </c>
@@ -6678,11 +6591,11 @@
         <f>Events!A12</f>
         <v>11th thing happened</v>
       </c>
-      <c r="B12" s="19" t="str">
+      <c r="B12" s="17" t="str">
         <f>TEXT(Events!B12, "MM/DD/YYYY")</f>
         <v>11/30/2014</v>
       </c>
-      <c r="C12" s="20" t="str">
+      <c r="C12" s="18" t="str">
         <f>TEXT(Events!C12, "HH:mm")</f>
         <v>11:00</v>
       </c>
@@ -6693,22 +6606,22 @@
       <c r="E12">
         <v>31.344614499999999</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <v>34.728752299999996</v>
       </c>
       <c r="G12" s="6" t="str">
         <f>Events!E12</f>
         <v>beta</v>
       </c>
-      <c r="H12" s="21" t="str">
+      <c r="H12" s="19" t="str">
         <f>IF(ISBLANK(Events!G12), "", Events!G12)</f>
         <v>narrative_3</v>
       </c>
-      <c r="I12" s="21" t="str">
+      <c r="I12" s="19" t="str">
         <f>IF(ISBLANK(Events!H12), "", Events!H12)</f>
         <v/>
       </c>
-      <c r="J12" s="21" t="str">
+      <c r="J12" s="19" t="str">
         <f>IF(ISBLANK(Events!I12), "", Events!I12)</f>
         <v>src8</v>
       </c>
@@ -6723,7 +6636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6739,10 +6652,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -6756,8 +6669,8 @@
         <f>Categories!B2</f>
         <v>Of highest priority</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="str">
@@ -6768,15 +6681,15 @@
         <f>Categories!B3</f>
         <v>Of lower priority</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -6798,28 +6711,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6831,7 +6744,7 @@
         <f>Sources!B2</f>
         <v>Gaza</v>
       </c>
-      <c r="C2" s="21" t="str">
+      <c r="C2" s="19" t="str">
         <f>IF(ISBLANK(Sources!C2), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C2))</f>
         <v/>
       </c>
@@ -6839,7 +6752,7 @@
         <f>Sources!D2</f>
         <v>Source 1 is a single photo.</v>
       </c>
-      <c r="E2" s="22" t="str">
+      <c r="E2" s="20" t="str">
         <f>IF(ISBLANK(Sources!E2), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E2))</f>
         <v>http://localhost:8000/source1.png</v>
       </c>
@@ -6865,7 +6778,7 @@
         <f>Sources!B3</f>
         <v>Spectrographs</v>
       </c>
-      <c r="C3" s="21" t="str">
+      <c r="C3" s="19" t="str">
         <f>IF(ISBLANK(Sources!C3), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C3))</f>
         <v/>
       </c>
@@ -6873,7 +6786,7 @@
         <f>Sources!D3</f>
         <v>Source 2 is a set of photos</v>
       </c>
-      <c r="E3" s="22" t="str">
+      <c r="E3" s="20" t="str">
         <f>IF(ISBLANK(Sources!E3), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E3))</f>
         <v>http://localhost:8000/source2/s1.jpg</v>
       </c>
@@ -6899,7 +6812,7 @@
         <f>Sources!B4</f>
         <v>Wacky</v>
       </c>
-      <c r="C4" s="21" t="str">
+      <c r="C4" s="19" t="str">
         <f>IF(ISBLANK(Sources!C4), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C4))</f>
         <v>http://localhost:8000/source2/s2.png</v>
       </c>
@@ -6907,7 +6820,7 @@
         <f>Sources!D4</f>
         <v>Source 3 is a video</v>
       </c>
-      <c r="E4" s="22" t="str">
+      <c r="E4" s="20" t="str">
         <f>IF(ISBLANK(Sources!E4), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E4))</f>
         <v>http://localhost:8000/source3.mp4</v>
       </c>
@@ -6933,7 +6846,7 @@
         <f>Sources!B5</f>
         <v>A Writeup for you</v>
       </c>
-      <c r="C5" s="21" t="str">
+      <c r="C5" s="19" t="str">
         <f>IF(ISBLANK(Sources!C5), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C5))</f>
         <v/>
       </c>
@@ -6941,7 +6854,7 @@
         <f>Sources!D5</f>
         <v>Source 4 is a text file</v>
       </c>
-      <c r="E5" s="22" t="str">
+      <c r="E5" s="20" t="str">
         <f>IF(ISBLANK(Sources!E5), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E5))</f>
         <v>http://localhost:8000/source4.md</v>
       </c>
@@ -6967,7 +6880,7 @@
         <f>Sources!B6</f>
         <v>kzm_hackhack-hack</v>
       </c>
-      <c r="C6" s="21" t="str">
+      <c r="C6" s="19" t="str">
         <f>IF(ISBLANK(Sources!C6), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C6))</f>
         <v>http://localhost:8000/source3/4.jpg</v>
       </c>
@@ -6975,7 +6888,7 @@
         <f>Sources!D6</f>
         <v>Source 5 is an erroneous source, as it includes a path with an unsupported file extension</v>
       </c>
-      <c r="E6" s="22" t="str">
+      <c r="E6" s="20" t="str">
         <f>IF(ISBLANK(Sources!E6), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E6))</f>
         <v>http://localhost:8000/source8.kzm</v>
       </c>
@@ -7001,7 +6914,7 @@
         <f>Sources!B7</f>
         <v>Can I Use a Video as a Thumbnail? Nope!</v>
       </c>
-      <c r="C7" s="21" t="str">
+      <c r="C7" s="19" t="str">
         <f>IF(ISBLANK(Sources!C7), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C7))</f>
         <v>http://localhost:8000/source3.mp4</v>
       </c>
@@ -7035,7 +6948,7 @@
         <f>Sources!B8</f>
         <v>A Composite Source. Image and Text</v>
       </c>
-      <c r="C8" s="21" t="str">
+      <c r="C8" s="19" t="str">
         <f>IF(ISBLANK(Sources!C8), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C8))</f>
         <v>http://localhost:8000/source2/s3.jpg</v>
       </c>
@@ -7043,7 +6956,7 @@
         <f>Sources!D8</f>
         <v>Source 7 is composed of both images and text.</v>
       </c>
-      <c r="E8" s="22" t="str">
+      <c r="E8" s="20" t="str">
         <f>IF(ISBLANK(Sources!E8), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E8))</f>
         <v>http://localhost:8000/source2/s3.jpg</v>
       </c>
@@ -7069,7 +6982,7 @@
         <f>Sources!B9</f>
         <v>A bad markdown source, to account for error handling.</v>
       </c>
-      <c r="C9" s="21" t="str">
+      <c r="C9" s="19" t="str">
         <f>IF(ISBLANK(Sources!C9), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C9))</f>
         <v>http://localhost:8000/source1.png</v>
       </c>
@@ -7077,7 +6990,7 @@
         <f>Sources!D9</f>
         <v>Source 8 begins with a bad markdown source.</v>
       </c>
-      <c r="E9" s="22" t="str">
+      <c r="E9" s="20" t="str">
         <f>IF(ISBLANK(Sources!E9), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E9))</f>
         <v>http://localhost:8000/non_existent.md</v>
       </c>
@@ -7093,6 +7006,164 @@
         <f>IF(ISBLANK(Sources!H9), "", Sources!H9)</f>
         <v/>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="str">
+        <f>Associations!A2</f>
+        <v>tear gas</v>
+      </c>
+      <c r="B2" s="6" t="str">
+        <f>Associations!B2</f>
+        <v>canisters</v>
+      </c>
+      <c r="C2" s="6" t="str">
+        <f>Associations!C2</f>
+        <v>Filter</v>
+      </c>
+      <c r="D2" s="6" t="str">
+        <f>Associations!D2</f>
+        <v>Weapons</v>
+      </c>
+      <c r="E2" s="6" t="str">
+        <f>Associations!E2</f>
+        <v>Close Range</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="str">
+        <f>Associations!A3</f>
+        <v>pistol</v>
+      </c>
+      <c r="B3" s="6" t="str">
+        <f>Associations!B3</f>
+        <v>gun</v>
+      </c>
+      <c r="C3" s="6" t="str">
+        <f>Associations!C3</f>
+        <v>Filter</v>
+      </c>
+      <c r="D3" s="6" t="str">
+        <f>Associations!D3</f>
+        <v>Weapons</v>
+      </c>
+      <c r="E3" s="6" t="str">
+        <f>Associations!E3</f>
+        <v>Long Range</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="str">
+        <f>Associations!A4</f>
+        <v>rifle</v>
+      </c>
+      <c r="B4" s="6" t="str">
+        <f>Associations!B4</f>
+        <v>gun</v>
+      </c>
+      <c r="C4" s="6" t="str">
+        <f>Associations!C4</f>
+        <v>Filter</v>
+      </c>
+      <c r="D4" s="6" t="str">
+        <f>Associations!D4</f>
+        <v>Weapons</v>
+      </c>
+      <c r="E4" s="6" t="str">
+        <f>Associations!E4</f>
+        <v>Long Range</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="str">
+        <f>Associations!A5</f>
+        <v>baton</v>
+      </c>
+      <c r="B5" s="6" t="str">
+        <f>Associations!B5</f>
+        <v>melee</v>
+      </c>
+      <c r="C5" s="6" t="str">
+        <f>Associations!C5</f>
+        <v>Filter</v>
+      </c>
+      <c r="D5" s="6" t="str">
+        <f>Associations!D5</f>
+        <v>Weapons</v>
+      </c>
+      <c r="E5" s="6" t="str">
+        <f>Associations!E5</f>
+        <v>Close Range</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="6" t="str">
+        <f>Associations!A6</f>
+        <v>narrative_1</v>
+      </c>
+      <c r="B6" s="6" t="str">
+        <f>Associations!B6</f>
+        <v>first narrative</v>
+      </c>
+      <c r="C6" s="6" t="str">
+        <f>Associations!C6</f>
+        <v>Narrative</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="6" t="str">
+        <f>Associations!A7</f>
+        <v>narrative_2</v>
+      </c>
+      <c r="B7" s="6" t="str">
+        <f>Associations!B7</f>
+        <v>second narrative</v>
+      </c>
+      <c r="C7" s="6" t="str">
+        <f>Associations!C7</f>
+        <v>Narrative</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Clean up with event related associations
</commit_message>
<xml_diff>
--- a/data/timemap_data.xlsx
+++ b/data/timemap_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/efarooqui/Desktop/FA/datasheet-server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4F17F0-39A3-7241-9580-2B1614C83EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6C354C-BD9E-704E-86E8-35631733B463}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="1640" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1197,7 +1197,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6173,7 +6173,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Spin up demo fixes
</commit_message>
<xml_diff>
--- a/data/timemap_data.xlsx
+++ b/data/timemap_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lachlankermode/code/_fa/datasheet-server/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juancamilogonzalez/dev/apps/datasheet-server/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14489D0E-9421-E54E-B57F-0B439F1F012E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABA0671-2726-9941-8EB2-09119F2244D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="24000" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" r:id="rId1"/>
@@ -306,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="128">
   <si>
     <t>Description</t>
   </si>
@@ -857,7 +857,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6083,7 +6083,7 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1:O1048576"/>
     </sheetView>
@@ -6942,10 +6942,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7090,40 +7090,6 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" t="s">
-        <v>103</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update source data to point to live URLs
</commit_message>
<xml_diff>
--- a/data/timemap_data.xlsx
+++ b/data/timemap_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Events" sheetId="1" state="visible" r:id="rId2"/>
@@ -126,56 +126,6 @@
           </rPr>
           <t xml:space="preserve">If the thumbnail is left blank and there are no images contained in the source, then an icon corresponding to the source type is used instead.
 	-Lachlan Kermode</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Non-existent thumbnail path
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">	-Lachlan Kermode</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Videos cannot be a thumbnail path: this source is also erroneous.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">	-Lachlan Kermode</t>
         </r>
       </text>
     </comment>
@@ -314,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="126">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -535,7 +485,7 @@
     <t xml:space="preserve">Source 1 is a single photo.</t>
   </si>
   <si>
-    <t xml:space="preserve">source1.png</t>
+    <t xml:space="preserve">https://image.shutterstock.com/image-photo/example-word-written-on-wooden-260nw-1765482248.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Photo</t>
@@ -547,13 +497,10 @@
     <t xml:space="preserve">Source 2 is a set of photos</t>
   </si>
   <si>
-    <t xml:space="preserve">source2/s1.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source2/s2.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source2/s3.jpg</t>
+    <t xml:space="preserve">https://cdn.pixabay.com/photo/2015/04/23/22/00/tree-736885__480.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/8/84/The_Bombing_of_Rafah.tif/lossless-page1-1200px-The_Bombing_of_Rafah.tif.png</t>
   </si>
   <si>
     <t xml:space="preserve">Photobook</t>
@@ -562,13 +509,10 @@
     <t xml:space="preserve">Wacky</t>
   </si>
   <si>
-    <t xml:space="preserve">source2/s2.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">Source 3 is a video</t>
   </si>
   <si>
-    <t xml:space="preserve">source3.mp4</t>
+    <t xml:space="preserve">https://datasheet-sources.ams3.digitaloceanspaces.com/ilovaisk_sources/Hromadske.tv%20-%20Paratroopers%20Video.mp4</t>
   </si>
   <si>
     <t xml:space="preserve">Video</t>
@@ -580,7 +524,7 @@
     <t xml:space="preserve">Source 4 is a text file</t>
   </si>
   <si>
-    <t xml:space="preserve">source4.md</t>
+    <t xml:space="preserve">https://d10yslqdemxz8r.cloudfront.net/welfare/nzherald-No-proof-of-abuse-by-doctor-say-police.md</t>
   </si>
   <si>
     <t xml:space="preserve">Eyewitness Testimony</t>
@@ -589,9 +533,6 @@
     <t xml:space="preserve">kzm_hackhack-hack</t>
   </si>
   <si>
-    <t xml:space="preserve">source3/4.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">Source 5 is an erroneous source, as it includes a path with an unsupported file extension</t>
   </si>
   <si>
@@ -604,6 +545,9 @@
     <t xml:space="preserve">Can I Use a Video as a Thumbnail? Nope!</t>
   </si>
   <si>
+    <t xml:space="preserve">https://file-examples-com.github.io/uploads/2017/04/file_example_MP4_480_1_5MG.mp4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Source 6 is another erroneous source: a video cannot be specified as a thumbnail. It is appropriate to include no paths in a source, so though the thumbnail should become an icon, the rest of the source should render correctly.</t>
   </si>
   <si>
@@ -659,9 +603,6 @@
   </si>
   <si>
     <t xml:space="preserve">association3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">association4</t>
   </si>
   <si>
     <t xml:space="preserve">source1</t>
@@ -716,7 +657,7 @@
     <numFmt numFmtId="169" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="170" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -785,6 +726,14 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -847,7 +796,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -909,6 +858,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -928,15 +881,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1019,11 +972,11 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.5"/>
@@ -5322,11 +5275,11 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.62890625" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.33"/>
   </cols>
@@ -5488,13 +5441,13 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="67.16"/>
@@ -5557,16 +5510,16 @@
         <v>76</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5574,21 +5527,21 @@
         <v>38</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5596,18 +5549,18 @@
         <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>86</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>88</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5615,19 +5568,19 @@
         <v>26</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5635,16 +5588,16 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5652,22 +5605,22 @@
         <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5675,19 +5628,19 @@
         <v>42</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5695,8 +5648,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId2" display="source4.md"/>
-    <hyperlink ref="F8" r:id="rId3" display="source4.md"/>
+    <hyperlink ref="E5" r:id="rId2" display="https://d10yslqdemxz8r.cloudfront.net/welfare/nzherald-No-proof-of-abuse-by-doctor-say-police.md"/>
+    <hyperlink ref="F8" r:id="rId3" display="https://d10yslqdemxz8r.cloudfront.net/welfare/nzherald-No-proof-of-abuse-by-doctor-say-police.md"/>
     <hyperlink ref="E9" r:id="rId4" display="non_existent.md"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5717,13 +5670,13 @@
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -5732,37 +5685,37 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5770,7 +5723,7 @@
         <v>63</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -5791,23 +5744,23 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>8</v>
@@ -5895,52 +5848,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.85" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5948,11 +5899,11 @@
         <f aca="false">Events!A2</f>
         <v>Person A appears on the scene and sprays tear gas.</v>
       </c>
-      <c r="B2" s="18" t="str">
+      <c r="B2" s="19" t="str">
         <f aca="false">TEXT(Events!B2, "MM/DD/YYYY")</f>
         <v>10/10/2015</v>
       </c>
-      <c r="C2" s="19" t="str">
+      <c r="C2" s="20" t="str">
         <f aca="false">TEXT(Events!C2, "HH:mm")</f>
         <v>16:20</v>
       </c>
@@ -5963,26 +5914,22 @@
       <c r="E2" s="0" t="n">
         <v>31.3484783</v>
       </c>
-      <c r="F2" s="20" t="n">
+      <c r="F2" s="21" t="n">
         <v>34.7874169</v>
       </c>
-      <c r="G2" s="21" t="str">
+      <c r="G2" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E2), "", Events!E2)</f>
         <v>tear_gas</v>
       </c>
-      <c r="H2" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I2" s="0" t="str">
+      <c r="H2" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F2), "", Events!F2)</f>
         <v>narrative_1</v>
       </c>
-      <c r="J2" s="0" t="str">
+      <c r="I2" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G2), "", Events!G2)</f>
         <v>narrative_3</v>
       </c>
-      <c r="K2" s="0" t="str">
+      <c r="J2" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H2), "", Events!H2)</f>
         <v>src1</v>
       </c>
@@ -5992,11 +5939,11 @@
         <f aca="false">Events!A3</f>
         <v>Person A begins recording, holding a pistol.</v>
       </c>
-      <c r="B3" s="18" t="str">
+      <c r="B3" s="19" t="str">
         <f aca="false">TEXT(Events!B3, "MM/DD/YYYY")</f>
         <v>10/10/2015</v>
       </c>
-      <c r="C3" s="19" t="str">
+      <c r="C3" s="20" t="str">
         <f aca="false">TEXT(Events!C3, "HH:mm")</f>
         <v>16:26</v>
       </c>
@@ -6007,26 +5954,22 @@
       <c r="E3" s="0" t="n">
         <v>31.3484783</v>
       </c>
-      <c r="F3" s="20" t="n">
+      <c r="F3" s="21" t="n">
         <v>34.7874169</v>
       </c>
-      <c r="G3" s="21" t="str">
+      <c r="G3" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E3), "", Events!E3)</f>
         <v>pistol</v>
       </c>
-      <c r="H3" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I3" s="0" t="str">
+      <c r="H3" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F3), "", Events!F3)</f>
         <v>narrative_1</v>
       </c>
-      <c r="J3" s="0" t="str">
+      <c r="I3" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G3), "", Events!G3)</f>
         <v>narrative_3</v>
       </c>
-      <c r="K3" s="0" t="str">
+      <c r="J3" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H3), "", Events!H3)</f>
         <v>src2</v>
       </c>
@@ -6036,11 +5979,11 @@
         <f aca="false">Events!A4</f>
         <v>Person B appears in Nahal Pehar, as captured by security footage, with a rifle.</v>
       </c>
-      <c r="B4" s="18" t="str">
+      <c r="B4" s="19" t="str">
         <f aca="false">TEXT(Events!B4, "MM/DD/YYYY")</f>
         <v>10/21/2015</v>
       </c>
-      <c r="C4" s="19" t="str">
+      <c r="C4" s="20" t="str">
         <f aca="false">TEXT(Events!C4, "HH:mm")</f>
         <v>07:00</v>
       </c>
@@ -6051,26 +5994,22 @@
       <c r="E4" s="0" t="n">
         <v>31.356397</v>
       </c>
-      <c r="F4" s="20" t="n">
+      <c r="F4" s="21" t="n">
         <v>34.784818</v>
       </c>
-      <c r="G4" s="21" t="str">
+      <c r="G4" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E4), "", Events!E4)</f>
         <v>rifle</v>
       </c>
-      <c r="H4" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I4" s="0" t="str">
+      <c r="H4" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F4), "", Events!F4)</f>
         <v>narrative_1</v>
       </c>
-      <c r="J4" s="0" t="str">
+      <c r="I4" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G4), "", Events!G4)</f>
         <v>narrative_3</v>
       </c>
-      <c r="K4" s="0" t="str">
+      <c r="J4" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H4), "", Events!H4)</f>
         <v>src6</v>
       </c>
@@ -6080,11 +6019,11 @@
         <f aca="false">Events!A5</f>
         <v>Fourth thing happened with a baton.</v>
       </c>
-      <c r="B5" s="18" t="str">
+      <c r="B5" s="19" t="str">
         <f aca="false">TEXT(Events!B5, "MM/DD/YYYY")</f>
         <v>10/08/2014</v>
       </c>
-      <c r="C5" s="19" t="str">
+      <c r="C5" s="20" t="str">
         <f aca="false">TEXT(Events!C5, "HH:mm")</f>
         <v>09:00</v>
       </c>
@@ -6095,26 +6034,22 @@
       <c r="E5" s="0" t="n">
         <v>31.3446145</v>
       </c>
-      <c r="F5" s="20" t="n">
+      <c r="F5" s="21" t="n">
         <v>34.7287523</v>
       </c>
-      <c r="G5" s="21" t="str">
+      <c r="G5" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E5), "", Events!E5)</f>
         <v>baton</v>
       </c>
-      <c r="H5" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I5" s="0" t="str">
+      <c r="H5" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F5), "", Events!F5)</f>
         <v>narrative_2</v>
       </c>
-      <c r="J5" s="0" t="str">
+      <c r="I5" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G5), "", Events!G5)</f>
         <v/>
       </c>
-      <c r="K5" s="0" t="str">
+      <c r="J5" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H5), "", Events!H5)</f>
         <v>src5</v>
       </c>
@@ -6124,11 +6059,11 @@
         <f aca="false">Events!A6</f>
         <v>Fifth thing happened with a baton.</v>
       </c>
-      <c r="B6" s="18" t="str">
+      <c r="B6" s="19" t="str">
         <f aca="false">TEXT(Events!B6, "MM/DD/YYYY")</f>
         <v>11/08/2014</v>
       </c>
-      <c r="C6" s="19" t="str">
+      <c r="C6" s="20" t="str">
         <f aca="false">TEXT(Events!C6, "HH:mm")</f>
         <v>09:00</v>
       </c>
@@ -6139,26 +6074,22 @@
       <c r="E6" s="0" t="n">
         <v>31.3640871</v>
       </c>
-      <c r="F6" s="20" t="n">
+      <c r="F6" s="21" t="n">
         <v>34.7135396</v>
       </c>
-      <c r="G6" s="21" t="str">
+      <c r="G6" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E6), "", Events!E6)</f>
         <v>baton</v>
       </c>
-      <c r="H6" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I6" s="0" t="str">
+      <c r="H6" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F6), "", Events!F6)</f>
         <v>narrative_2</v>
       </c>
-      <c r="J6" s="0" t="str">
+      <c r="I6" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G6), "", Events!G6)</f>
         <v/>
       </c>
-      <c r="K6" s="0" t="str">
+      <c r="J6" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H6), "", Events!H6)</f>
         <v>src7</v>
       </c>
@@ -6168,11 +6099,11 @@
         <f aca="false">Events!A7</f>
         <v>Sixth thing happened with a rifle.</v>
       </c>
-      <c r="B7" s="18" t="str">
+      <c r="B7" s="19" t="str">
         <f aca="false">TEXT(Events!B7, "MM/DD/YYYY")</f>
         <v>12/09/2014</v>
       </c>
-      <c r="C7" s="19" t="str">
+      <c r="C7" s="20" t="str">
         <f aca="false">TEXT(Events!C7, "HH:mm")</f>
         <v>12:00</v>
       </c>
@@ -6183,26 +6114,22 @@
       <c r="E7" s="0" t="n">
         <v>31.3440514</v>
       </c>
-      <c r="F7" s="20" t="n">
+      <c r="F7" s="21" t="n">
         <v>34.7616005</v>
       </c>
-      <c r="G7" s="21" t="str">
+      <c r="G7" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E7), "", Events!E7)</f>
         <v>rifle</v>
       </c>
-      <c r="H7" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I7" s="0" t="str">
+      <c r="H7" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F7), "", Events!F7)</f>
         <v>narrative_2</v>
       </c>
-      <c r="J7" s="0" t="str">
+      <c r="I7" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G7), "", Events!G7)</f>
         <v/>
       </c>
-      <c r="K7" s="0" t="str">
+      <c r="J7" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H7), "", Events!H7)</f>
         <v>src7</v>
       </c>
@@ -6212,32 +6139,28 @@
         <f aca="false">Events!A8</f>
         <v>Somthing happened (out of space); i.e. some legislation passed regarding pistols.</v>
       </c>
-      <c r="B8" s="18" t="str">
+      <c r="B8" s="19" t="str">
         <f aca="false">TEXT(Events!B8, "MM/DD/YYYY")</f>
         <v>12/10/2014</v>
       </c>
-      <c r="C8" s="19" t="str">
+      <c r="C8" s="20" t="str">
         <f aca="false">TEXT(Events!C8, "HH:mm")</f>
         <v>01:00</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21" t="str">
+      <c r="F8" s="21"/>
+      <c r="G8" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E8), "", Events!E8)</f>
         <v>pistol</v>
       </c>
-      <c r="H8" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I8" s="0" t="str">
+      <c r="H8" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F8), "", Events!F8)</f>
         <v>narrative_3</v>
       </c>
-      <c r="J8" s="0" t="str">
+      <c r="I8" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G8), "", Events!G8)</f>
         <v/>
       </c>
-      <c r="K8" s="0" t="str">
+      <c r="J8" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H8), "", Events!H8)</f>
         <v>src4</v>
       </c>
@@ -6247,11 +6170,11 @@
         <f aca="false">Events!A9</f>
         <v>8th thing happened, and there was tear gas.</v>
       </c>
-      <c r="B9" s="18" t="str">
+      <c r="B9" s="19" t="str">
         <f aca="false">TEXT(Events!B9, "MM/DD/YYYY")</f>
         <v>12/09/2014</v>
       </c>
-      <c r="C9" s="19" t="str">
+      <c r="C9" s="20" t="str">
         <f aca="false">TEXT(Events!C9, "HH:mm")</f>
         <v>11:00</v>
       </c>
@@ -6262,26 +6185,22 @@
       <c r="E9" s="0" t="n">
         <v>31.3424027</v>
       </c>
-      <c r="F9" s="20" t="n">
+      <c r="F9" s="21" t="n">
         <v>34.7909811</v>
       </c>
-      <c r="G9" s="21" t="str">
+      <c r="G9" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E9), "", Events!E9)</f>
         <v>tear_gas</v>
       </c>
-      <c r="H9" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I9" s="0" t="str">
+      <c r="H9" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F9), "", Events!F9)</f>
         <v>narrative_1</v>
       </c>
-      <c r="J9" s="0" t="str">
+      <c r="I9" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G9), "", Events!G9)</f>
         <v/>
       </c>
-      <c r="K9" s="0" t="str">
+      <c r="J9" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H9), "", Events!H9)</f>
         <v>src5</v>
       </c>
@@ -6291,11 +6210,11 @@
         <f aca="false">Events!A10</f>
         <v>9th thing happened</v>
       </c>
-      <c r="B10" s="18" t="str">
+      <c r="B10" s="19" t="str">
         <f aca="false">TEXT(Events!B10, "MM/DD/YYYY")</f>
         <v>12/09/2014</v>
       </c>
-      <c r="C10" s="19" t="str">
+      <c r="C10" s="20" t="str">
         <f aca="false">TEXT(Events!C10, "HH:mm")</f>
         <v>11:00</v>
       </c>
@@ -6306,26 +6225,22 @@
       <c r="E10" s="0" t="n">
         <v>31.356397</v>
       </c>
-      <c r="F10" s="20" t="n">
+      <c r="F10" s="21" t="n">
         <v>34.784818</v>
       </c>
-      <c r="G10" s="21" t="str">
+      <c r="G10" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E10), "", Events!E10)</f>
         <v/>
       </c>
-      <c r="H10" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I10" s="0" t="str">
+      <c r="H10" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F10), "", Events!F10)</f>
         <v>narrative_2</v>
       </c>
-      <c r="J10" s="0" t="str">
+      <c r="I10" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G10), "", Events!G10)</f>
         <v/>
       </c>
-      <c r="K10" s="0" t="str">
+      <c r="J10" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H10), "", Events!H10)</f>
         <v>src3</v>
       </c>
@@ -6335,11 +6250,11 @@
         <f aca="false">Events!A11</f>
         <v>10th thing happened</v>
       </c>
-      <c r="B11" s="18" t="str">
+      <c r="B11" s="19" t="str">
         <f aca="false">TEXT(Events!B11, "MM/DD/YYYY")</f>
         <v>11/09/2014</v>
       </c>
-      <c r="C11" s="19" t="str">
+      <c r="C11" s="20" t="str">
         <f aca="false">TEXT(Events!C11, "HH:mm")</f>
         <v>10:48</v>
       </c>
@@ -6350,26 +6265,22 @@
       <c r="E11" s="0" t="n">
         <v>31.356397</v>
       </c>
-      <c r="F11" s="20" t="n">
+      <c r="F11" s="21" t="n">
         <v>34.784818</v>
       </c>
-      <c r="G11" s="21" t="str">
+      <c r="G11" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E11), "", Events!E11)</f>
         <v/>
       </c>
-      <c r="H11" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I11" s="0" t="str">
+      <c r="H11" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F11), "", Events!F11)</f>
         <v/>
       </c>
-      <c r="J11" s="0" t="str">
+      <c r="I11" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G11), "", Events!G11)</f>
         <v/>
       </c>
-      <c r="K11" s="0" t="str">
+      <c r="J11" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H11), "", Events!H11)</f>
         <v>src6</v>
       </c>
@@ -6379,11 +6290,11 @@
         <f aca="false">Events!A12</f>
         <v>11th thing happened</v>
       </c>
-      <c r="B12" s="18" t="str">
+      <c r="B12" s="19" t="str">
         <f aca="false">TEXT(Events!B12, "MM/DD/YYYY")</f>
         <v>11/30/2014</v>
       </c>
-      <c r="C12" s="19" t="str">
+      <c r="C12" s="20" t="str">
         <f aca="false">TEXT(Events!C12, "HH:mm")</f>
         <v>11:00</v>
       </c>
@@ -6394,26 +6305,22 @@
       <c r="E12" s="0" t="n">
         <v>31.3446145</v>
       </c>
-      <c r="F12" s="20" t="n">
+      <c r="F12" s="21" t="n">
         <v>34.7287523</v>
       </c>
-      <c r="G12" s="21" t="str">
+      <c r="G12" s="22" t="str">
         <f aca="false">IF(ISBLANK(Events!E12), "", Events!E12)</f>
         <v/>
       </c>
-      <c r="H12" s="21" t="e">
-        <f aca="false">IF(ISBLANK(#REF!), "", #REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I12" s="0" t="str">
+      <c r="H12" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!F12), "", Events!F12)</f>
         <v>narrative_3</v>
       </c>
-      <c r="J12" s="0" t="str">
+      <c r="I12" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!G12), "", Events!G12)</f>
         <v/>
       </c>
-      <c r="K12" s="0" t="str">
+      <c r="J12" s="0" t="str">
         <f aca="false">IF(ISBLANK(Events!H12), "", Events!H12)</f>
         <v>src8</v>
       </c>
@@ -6437,13 +6344,13 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.83"/>
@@ -6453,28 +6360,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6486,7 +6393,7 @@
         <f aca="false">Sources!B2</f>
         <v>Gaza</v>
       </c>
-      <c r="C2" s="21" t="str">
+      <c r="C2" s="22" t="str">
         <f aca="false">IF(ISBLANK(Sources!C2), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C2))</f>
         <v/>
       </c>
@@ -6494,9 +6401,9 @@
         <f aca="false">Sources!D2</f>
         <v>Source 1 is a single photo.</v>
       </c>
-      <c r="E2" s="22" t="str">
+      <c r="E2" s="23" t="str">
         <f aca="false">IF(ISBLANK(Sources!E2), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E2))</f>
-        <v>http://localhost:8000/source1.png</v>
+        <v>http://localhost:8000/https://image.shutterstock.com/image-photo/example-word-written-on-wooden-260nw-1765482248.jpg</v>
       </c>
       <c r="F2" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!F2), "", _xlfn.CONCAT("http://localhost:8000/", Sources!F2))</f>
@@ -6520,7 +6427,7 @@
         <f aca="false">Sources!B3</f>
         <v>Spectrographs</v>
       </c>
-      <c r="C3" s="21" t="str">
+      <c r="C3" s="22" t="str">
         <f aca="false">IF(ISBLANK(Sources!C3), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C3))</f>
         <v/>
       </c>
@@ -6528,17 +6435,17 @@
         <f aca="false">Sources!D3</f>
         <v>Source 2 is a set of photos</v>
       </c>
-      <c r="E3" s="22" t="str">
+      <c r="E3" s="23" t="str">
         <f aca="false">IF(ISBLANK(Sources!E3), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E3))</f>
-        <v>http://localhost:8000/source2/s1.jpg</v>
+        <v>http://localhost:8000/https://image.shutterstock.com/image-photo/example-word-written-on-wooden-260nw-1765482248.jpg</v>
       </c>
       <c r="F3" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!F3), "", _xlfn.CONCAT("http://localhost:8000/", Sources!F3))</f>
-        <v>http://localhost:8000/source2/s2.jpg</v>
+        <v>http://localhost:8000/https://cdn.pixabay.com/photo/2015/04/23/22/00/tree-736885__480.jpg</v>
       </c>
       <c r="G3" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!G3), "", _xlfn.CONCAT("http://localhost:8000/", Sources!G3))</f>
-        <v>http://localhost:8000/source2/s3.jpg</v>
+        <v>http://localhost:8000/https://upload.wikimedia.org/wikipedia/commons/thumb/8/84/The_Bombing_of_Rafah.tif/lossless-page1-1200px-The_Bombing_of_Rafah.tif.png</v>
       </c>
       <c r="H3" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!H3), "", Sources!H3)</f>
@@ -6554,17 +6461,17 @@
         <f aca="false">Sources!B4</f>
         <v>Wacky</v>
       </c>
-      <c r="C4" s="21" t="str">
+      <c r="C4" s="22" t="str">
         <f aca="false">IF(ISBLANK(Sources!C4), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C4))</f>
-        <v>http://localhost:8000/source2/s2.png</v>
+        <v>http://localhost:8000/https://cdn.pixabay.com/photo/2015/04/23/22/00/tree-736885__480.jpg</v>
       </c>
       <c r="D4" s="0" t="str">
         <f aca="false">Sources!D4</f>
         <v>Source 3 is a video</v>
       </c>
-      <c r="E4" s="22" t="str">
+      <c r="E4" s="23" t="str">
         <f aca="false">IF(ISBLANK(Sources!E4), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E4))</f>
-        <v>http://localhost:8000/source3.mp4</v>
+        <v>http://localhost:8000/https://datasheet-sources.ams3.digitaloceanspaces.com/ilovaisk_sources/Hromadske.tv%20-%20Paratroopers%20Video.mp4</v>
       </c>
       <c r="F4" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!F4), "", _xlfn.CONCAT("http://localhost:8000/", Sources!F4))</f>
@@ -6588,7 +6495,7 @@
         <f aca="false">Sources!B5</f>
         <v>A Writeup for you</v>
       </c>
-      <c r="C5" s="21" t="str">
+      <c r="C5" s="22" t="str">
         <f aca="false">IF(ISBLANK(Sources!C5), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C5))</f>
         <v/>
       </c>
@@ -6596,9 +6503,9 @@
         <f aca="false">Sources!D5</f>
         <v>Source 4 is a text file</v>
       </c>
-      <c r="E5" s="22" t="str">
+      <c r="E5" s="23" t="str">
         <f aca="false">IF(ISBLANK(Sources!E5), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E5))</f>
-        <v>http://localhost:8000/source4.md</v>
+        <v>http://localhost:8000/https://d10yslqdemxz8r.cloudfront.net/welfare/nzherald-No-proof-of-abuse-by-doctor-say-police.md</v>
       </c>
       <c r="F5" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!F5), "", _xlfn.CONCAT("http://localhost:8000/", Sources!F5))</f>
@@ -6622,15 +6529,15 @@
         <f aca="false">Sources!B6</f>
         <v>kzm_hackhack-hack</v>
       </c>
-      <c r="C6" s="21" t="str">
+      <c r="C6" s="22" t="str">
         <f aca="false">IF(ISBLANK(Sources!C6), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C6))</f>
-        <v>http://localhost:8000/source3/4.jpg</v>
+        <v>http://localhost:8000/https://image.shutterstock.com/image-photo/example-word-written-on-wooden-260nw-1765482248.jpg</v>
       </c>
       <c r="D6" s="0" t="str">
         <f aca="false">Sources!D6</f>
         <v>Source 5 is an erroneous source, as it includes a path with an unsupported file extension</v>
       </c>
-      <c r="E6" s="22" t="str">
+      <c r="E6" s="23" t="str">
         <f aca="false">IF(ISBLANK(Sources!E6), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E6))</f>
         <v>http://localhost:8000/source8.kzm</v>
       </c>
@@ -6656,9 +6563,9 @@
         <f aca="false">Sources!B7</f>
         <v>Can I Use a Video as a Thumbnail? Nope!</v>
       </c>
-      <c r="C7" s="21" t="str">
+      <c r="C7" s="22" t="str">
         <f aca="false">IF(ISBLANK(Sources!C7), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C7))</f>
-        <v>http://localhost:8000/source3.mp4</v>
+        <v>http://localhost:8000/https://file-examples-com.github.io/uploads/2017/04/file_example_MP4_480_1_5MG.mp4</v>
       </c>
       <c r="D7" s="0" t="str">
         <f aca="false">Sources!D7</f>
@@ -6690,21 +6597,21 @@
         <f aca="false">Sources!B8</f>
         <v>A Composite Source. Image and Text</v>
       </c>
-      <c r="C8" s="21" t="str">
+      <c r="C8" s="22" t="str">
         <f aca="false">IF(ISBLANK(Sources!C8), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C8))</f>
-        <v>http://localhost:8000/source2/s3.jpg</v>
+        <v>http://localhost:8000/https://image.shutterstock.com/image-photo/example-word-written-on-wooden-260nw-1765482248.jpg</v>
       </c>
       <c r="D8" s="0" t="str">
         <f aca="false">Sources!D8</f>
         <v>Source 7 is composed of both images and text.</v>
       </c>
-      <c r="E8" s="22" t="str">
+      <c r="E8" s="23" t="str">
         <f aca="false">IF(ISBLANK(Sources!E8), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E8))</f>
-        <v>http://localhost:8000/source2/s3.jpg</v>
+        <v>http://localhost:8000/https://upload.wikimedia.org/wikipedia/commons/thumb/8/84/The_Bombing_of_Rafah.tif/lossless-page1-1200px-The_Bombing_of_Rafah.tif.png</v>
       </c>
       <c r="F8" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!F8), "", _xlfn.CONCAT("http://localhost:8000/", Sources!F8))</f>
-        <v>http://localhost:8000/source4.md</v>
+        <v>http://localhost:8000/https://d10yslqdemxz8r.cloudfront.net/welfare/nzherald-No-proof-of-abuse-by-doctor-say-police.md</v>
       </c>
       <c r="G8" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!G8), "", _xlfn.CONCAT("http://localhost:8000/", Sources!G8))</f>
@@ -6724,21 +6631,21 @@
         <f aca="false">Sources!B9</f>
         <v>A bad markdown source, to account for error handling.</v>
       </c>
-      <c r="C9" s="21" t="str">
+      <c r="C9" s="22" t="str">
         <f aca="false">IF(ISBLANK(Sources!C9), "", _xlfn.CONCAT("http://localhost:8000/", Sources!C9))</f>
-        <v>http://localhost:8000/source1.png</v>
+        <v>http://localhost:8000/https://image.shutterstock.com/image-photo/example-word-written-on-wooden-260nw-1765482248.jpg</v>
       </c>
       <c r="D9" s="0" t="str">
         <f aca="false">Sources!D9</f>
         <v>Source 8 begins with a bad markdown source.</v>
       </c>
-      <c r="E9" s="22" t="str">
+      <c r="E9" s="23" t="str">
         <f aca="false">IF(ISBLANK(Sources!E9), "", _xlfn.CONCAT("http://localhost:8000/", Sources!E9))</f>
         <v>http://localhost:8000/non_existent.md</v>
       </c>
       <c r="F9" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!F9), "", _xlfn.CONCAT("http://localhost:8000/", Sources!F9))</f>
-        <v>http://localhost:8000/source1.png</v>
+        <v>http://localhost:8000/https://upload.wikimedia.org/wikipedia/commons/thumb/8/84/The_Bombing_of_Rafah.tif/lossless-page1-1200px-The_Bombing_of_Rafah.tif.png</v>
       </c>
       <c r="G9" s="0" t="str">
         <f aca="false">IF(ISBLANK(Sources!G9), "", _xlfn.CONCAT("http://localhost:8000/", Sources!G9))</f>
@@ -6911,33 +6818,33 @@
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="13" t="s">
         <v>125</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>